<commit_message>
data driven test cases
</commit_message>
<xml_diff>
--- a/EtsyCommerce/testData/TestData.xlsx
+++ b/EtsyCommerce/testData/TestData.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marzana\Desktop\SelFrameworkGroup4\EtsyCommerce\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADF770C-8A47-4FBA-8AAF-1A82C8AFF3FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638E3090-F20B-434B-98A6-5CC477B2A40D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4350" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -31,39 +30,18 @@
     <t>password</t>
   </si>
   <si>
-    <t>expectedErroMessage</t>
-  </si>
-  <si>
     <t>jah@gmail.com</t>
   </si>
   <si>
-    <t>abcd@gmail.com</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>xyz@gmail.com</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>hello</t>
   </si>
   <si>
-    <t>There is 1 error</t>
-  </si>
-  <si>
     <t>jggg@gmail.com</t>
   </si>
   <si>
     <t>Hi3345</t>
   </si>
   <si>
-    <t>asdf@gmail.com</t>
-  </si>
-  <si>
     <t>H1234</t>
   </si>
   <si>
@@ -80,13 +58,34 @@
   </si>
   <si>
     <t>H1233</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is a gift card. </t>
+  </si>
+  <si>
+    <t>bob@gmail.com</t>
+  </si>
+  <si>
+    <t>H1232@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -100,11 +99,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
     </font>
     <font>
       <u/>
@@ -145,26 +139,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,236 +467,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3409AAF-B24E-4B18-859D-ED340BF5805A}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A26966EE-BB91-46E9-A24D-B38AA9668830}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD23DC3-65F2-4CFF-BEFF-466E881D1F79}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="65.85546875" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{98FDDFD2-2DDB-49D3-ADE3-0B73DE5FC4E4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741C5EB8-08E2-4AE9-A022-E1FD0767E3EA}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>